<commit_message>
Atualização do código da anfavea por questão de erros
</commit_message>
<xml_diff>
--- a/Arquivo/emplacamento.xlsx
+++ b/Arquivo/emplacamento.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Estat\DESEMP23\ArquivosParaSite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D33B56-BF4D-4201-9D45-DDF970C17EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA30E86-29B8-4216-AA42-5431648C3421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1281,9 +1281,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1321,9 +1321,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1356,26 +1356,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1408,26 +1391,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1691,8 +1657,8 @@
   </sheetPr>
   <dimension ref="B2:T65"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,7 +1796,7 @@
         <v>149064</v>
       </c>
       <c r="I7" s="20">
-        <v>0</v>
+        <v>161611</v>
       </c>
       <c r="J7" s="20">
         <v>0</v>
@@ -1851,7 +1817,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="20">
-        <v>693417</v>
+        <v>855028</v>
       </c>
       <c r="Q7" s="3"/>
     </row>
@@ -1876,7 +1842,7 @@
         <v>139615</v>
       </c>
       <c r="I8" s="21">
-        <v>0</v>
+        <v>152415</v>
       </c>
       <c r="J8" s="21">
         <v>0</v>
@@ -1897,7 +1863,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="21">
-        <v>643077</v>
+        <v>795492</v>
       </c>
       <c r="Q8" s="3"/>
     </row>
@@ -1922,7 +1888,7 @@
         <v>110168</v>
       </c>
       <c r="I9" s="15">
-        <v>0</v>
+        <v>123321</v>
       </c>
       <c r="J9" s="15">
         <v>0</v>
@@ -1943,7 +1909,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="15">
-        <v>521583</v>
+        <v>644904</v>
       </c>
       <c r="Q9" s="3"/>
     </row>
@@ -1968,7 +1934,7 @@
         <v>29447</v>
       </c>
       <c r="I10" s="15">
-        <v>0</v>
+        <v>29094</v>
       </c>
       <c r="J10" s="15">
         <v>0</v>
@@ -1989,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="15">
-        <v>121494</v>
+        <v>150588</v>
       </c>
       <c r="Q10" s="3"/>
     </row>
@@ -2014,7 +1980,7 @@
         <v>7529</v>
       </c>
       <c r="I11" s="21">
-        <v>0</v>
+        <v>7422</v>
       </c>
       <c r="J11" s="21">
         <v>0</v>
@@ -2035,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="21">
-        <v>40798</v>
+        <v>48220</v>
       </c>
       <c r="Q11" s="3"/>
     </row>
@@ -2060,7 +2026,7 @@
         <v>124</v>
       </c>
       <c r="I12" s="15">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="J12" s="15">
         <v>0</v>
@@ -2081,7 +2047,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="15">
-        <v>457</v>
+        <v>529</v>
       </c>
       <c r="Q12" s="3"/>
     </row>
@@ -2106,7 +2072,7 @@
         <v>675</v>
       </c>
       <c r="I13" s="15">
-        <v>0</v>
+        <v>652</v>
       </c>
       <c r="J13" s="15">
         <v>0</v>
@@ -2127,7 +2093,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="15">
-        <v>3716</v>
+        <v>4368</v>
       </c>
       <c r="Q13" s="3"/>
     </row>
@@ -2152,7 +2118,7 @@
         <v>721</v>
       </c>
       <c r="I14" s="15">
-        <v>0</v>
+        <v>645</v>
       </c>
       <c r="J14" s="15">
         <v>0</v>
@@ -2173,7 +2139,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="15">
-        <v>3589</v>
+        <v>4234</v>
       </c>
       <c r="Q14" s="3"/>
     </row>
@@ -2198,7 +2164,7 @@
         <v>2284</v>
       </c>
       <c r="I15" s="15">
-        <v>0</v>
+        <v>2127</v>
       </c>
       <c r="J15" s="15">
         <v>0</v>
@@ -2219,7 +2185,7 @@
         <v>0</v>
       </c>
       <c r="P15" s="15">
-        <v>12066</v>
+        <v>14193</v>
       </c>
       <c r="Q15" s="3"/>
     </row>
@@ -2244,7 +2210,7 @@
         <v>3725</v>
       </c>
       <c r="I16" s="15">
-        <v>0</v>
+        <v>3926</v>
       </c>
       <c r="J16" s="15">
         <v>0</v>
@@ -2265,7 +2231,7 @@
         <v>0</v>
       </c>
       <c r="P16" s="15">
-        <v>20970</v>
+        <v>24896</v>
       </c>
       <c r="Q16" s="3"/>
     </row>
@@ -2290,7 +2256,7 @@
         <v>1920</v>
       </c>
       <c r="I17" s="22">
-        <v>0</v>
+        <v>1774</v>
       </c>
       <c r="J17" s="22">
         <v>0</v>
@@ -2311,7 +2277,7 @@
         <v>0</v>
       </c>
       <c r="P17" s="22">
-        <v>9542</v>
+        <v>11316</v>
       </c>
       <c r="Q17" s="3"/>
     </row>
@@ -2448,7 +2414,7 @@
         <v>27460</v>
       </c>
       <c r="I26" s="20">
-        <v>0</v>
+        <v>27917</v>
       </c>
       <c r="J26" s="20">
         <v>0</v>
@@ -2469,7 +2435,7 @@
         <v>0</v>
       </c>
       <c r="P26" s="20">
-        <v>115612</v>
+        <v>143529</v>
       </c>
       <c r="Q26" s="3"/>
     </row>
@@ -2494,7 +2460,7 @@
         <v>26766</v>
       </c>
       <c r="I27" s="21">
-        <v>0</v>
+        <v>27455</v>
       </c>
       <c r="J27" s="21">
         <v>0</v>
@@ -2515,7 +2481,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="21">
-        <v>111741</v>
+        <v>139196</v>
       </c>
       <c r="Q27" s="3"/>
     </row>
@@ -2540,7 +2506,7 @@
         <v>17340</v>
       </c>
       <c r="I28" s="15">
-        <v>0</v>
+        <v>18716</v>
       </c>
       <c r="J28" s="15">
         <v>0</v>
@@ -2561,7 +2527,7 @@
         <v>0</v>
       </c>
       <c r="P28" s="21">
-        <v>70095</v>
+        <v>88811</v>
       </c>
       <c r="Q28" s="3"/>
     </row>
@@ -2586,7 +2552,7 @@
         <v>9426</v>
       </c>
       <c r="I29" s="15">
-        <v>0</v>
+        <v>8739</v>
       </c>
       <c r="J29" s="15">
         <v>0</v>
@@ -2607,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="P29" s="21">
-        <v>41646</v>
+        <v>50385</v>
       </c>
       <c r="Q29" s="3"/>
     </row>
@@ -2632,7 +2598,7 @@
         <v>694</v>
       </c>
       <c r="I30" s="21">
-        <v>0</v>
+        <v>462</v>
       </c>
       <c r="J30" s="21">
         <v>0</v>
@@ -2653,7 +2619,7 @@
         <v>0</v>
       </c>
       <c r="P30" s="21">
-        <v>3865</v>
+        <v>4327</v>
       </c>
       <c r="Q30" s="3"/>
     </row>
@@ -2678,7 +2644,7 @@
         <v>649</v>
       </c>
       <c r="I31" s="15">
-        <v>0</v>
+        <v>440</v>
       </c>
       <c r="J31" s="15">
         <v>0</v>
@@ -2699,7 +2665,7 @@
         <v>0</v>
       </c>
       <c r="P31" s="21">
-        <v>3602</v>
+        <v>4042</v>
       </c>
       <c r="Q31" s="3"/>
     </row>
@@ -2724,7 +2690,7 @@
         <v>23</v>
       </c>
       <c r="I32" s="15">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J32" s="15">
         <v>0</v>
@@ -2745,7 +2711,7 @@
         <v>0</v>
       </c>
       <c r="P32" s="21">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="Q32" s="3"/>
     </row>
@@ -2770,7 +2736,7 @@
         <v>20</v>
       </c>
       <c r="I33" s="15">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J33" s="15">
         <v>0</v>
@@ -2791,7 +2757,7 @@
         <v>0</v>
       </c>
       <c r="P33" s="21">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="Q33" s="3"/>
     </row>
@@ -2816,7 +2782,7 @@
         <v>0</v>
       </c>
       <c r="I34" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J34" s="15">
         <v>0</v>
@@ -2837,7 +2803,7 @@
         <v>0</v>
       </c>
       <c r="P34" s="21">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q34" s="3"/>
     </row>
@@ -2862,7 +2828,7 @@
         <v>2</v>
       </c>
       <c r="I35" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" s="15">
         <v>0</v>
@@ -2883,7 +2849,7 @@
         <v>0</v>
       </c>
       <c r="P35" s="21">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q35" s="3"/>
     </row>
@@ -3066,7 +3032,7 @@
         <v>176524</v>
       </c>
       <c r="I45" s="20">
-        <v>0</v>
+        <v>189528</v>
       </c>
       <c r="J45" s="20">
         <v>0</v>
@@ -3087,7 +3053,7 @@
         <v>0</v>
       </c>
       <c r="P45" s="20">
-        <v>809029</v>
+        <v>998557</v>
       </c>
       <c r="Q45" s="3"/>
     </row>
@@ -3112,7 +3078,7 @@
         <v>166381</v>
       </c>
       <c r="I46" s="21">
-        <v>0</v>
+        <v>179870</v>
       </c>
       <c r="J46" s="21">
         <v>0</v>
@@ -3133,7 +3099,7 @@
         <v>0</v>
       </c>
       <c r="P46" s="21">
-        <v>754818</v>
+        <v>934688</v>
       </c>
       <c r="Q46" s="3"/>
     </row>
@@ -3158,7 +3124,7 @@
         <v>127508</v>
       </c>
       <c r="I47" s="15">
-        <v>0</v>
+        <v>142037</v>
       </c>
       <c r="J47" s="15">
         <v>0</v>
@@ -3179,7 +3145,7 @@
         <v>0</v>
       </c>
       <c r="P47" s="15">
-        <v>591678</v>
+        <v>733715</v>
       </c>
       <c r="Q47" s="3"/>
     </row>
@@ -3204,7 +3170,7 @@
         <v>38873</v>
       </c>
       <c r="I48" s="15">
-        <v>0</v>
+        <v>37833</v>
       </c>
       <c r="J48" s="15">
         <v>0</v>
@@ -3225,7 +3191,7 @@
         <v>0</v>
       </c>
       <c r="P48" s="15">
-        <v>163140</v>
+        <v>200973</v>
       </c>
       <c r="Q48" s="3"/>
     </row>
@@ -3250,7 +3216,7 @@
         <v>8223</v>
       </c>
       <c r="I49" s="21">
-        <v>0</v>
+        <v>7884</v>
       </c>
       <c r="J49" s="21">
         <v>0</v>
@@ -3271,7 +3237,7 @@
         <v>0</v>
       </c>
       <c r="P49" s="21">
-        <v>44663</v>
+        <v>52547</v>
       </c>
       <c r="Q49" s="3"/>
     </row>
@@ -3296,7 +3262,7 @@
         <v>773</v>
       </c>
       <c r="I50" s="15">
-        <v>0</v>
+        <v>512</v>
       </c>
       <c r="J50" s="15">
         <v>0</v>
@@ -3317,7 +3283,7 @@
         <v>0</v>
       </c>
       <c r="P50" s="15">
-        <v>4059</v>
+        <v>4571</v>
       </c>
       <c r="Q50" s="3"/>
     </row>
@@ -3342,7 +3308,7 @@
         <v>698</v>
       </c>
       <c r="I51" s="15">
-        <v>0</v>
+        <v>658</v>
       </c>
       <c r="J51" s="15">
         <v>0</v>
@@ -3363,7 +3329,7 @@
         <v>0</v>
       </c>
       <c r="P51" s="15">
-        <v>3887</v>
+        <v>4545</v>
       </c>
       <c r="Q51" s="3"/>
     </row>
@@ -3388,7 +3354,7 @@
         <v>741</v>
       </c>
       <c r="I52" s="15">
-        <v>0</v>
+        <v>658</v>
       </c>
       <c r="J52" s="15">
         <v>0</v>
@@ -3409,7 +3375,7 @@
         <v>0</v>
       </c>
       <c r="P52" s="15">
-        <v>3659</v>
+        <v>4317</v>
       </c>
       <c r="Q52" s="3"/>
     </row>
@@ -3434,7 +3400,7 @@
         <v>2284</v>
       </c>
       <c r="I53" s="15">
-        <v>0</v>
+        <v>2129</v>
       </c>
       <c r="J53" s="15">
         <v>0</v>
@@ -3455,7 +3421,7 @@
         <v>0</v>
       </c>
       <c r="P53" s="15">
-        <v>12074</v>
+        <v>14203</v>
       </c>
       <c r="Q53" s="3"/>
     </row>
@@ -3480,7 +3446,7 @@
         <v>3727</v>
       </c>
       <c r="I54" s="15">
-        <v>0</v>
+        <v>3927</v>
       </c>
       <c r="J54" s="15">
         <v>0</v>
@@ -3501,7 +3467,7 @@
         <v>0</v>
       </c>
       <c r="P54" s="15">
-        <v>20984</v>
+        <v>24911</v>
       </c>
       <c r="Q54" s="3"/>
     </row>
@@ -3526,7 +3492,7 @@
         <v>1920</v>
       </c>
       <c r="I55" s="22">
-        <v>0</v>
+        <v>1774</v>
       </c>
       <c r="J55" s="22">
         <v>0</v>
@@ -3547,7 +3513,7 @@
         <v>0</v>
       </c>
       <c r="P55" s="43">
-        <v>9548</v>
+        <v>11322</v>
       </c>
       <c r="Q55" s="3"/>
     </row>
@@ -3710,7 +3676,7 @@
         <v>15.555958396591965</v>
       </c>
       <c r="I63" s="55">
-        <v>0</v>
+        <v>14.729749693976615</v>
       </c>
       <c r="J63" s="55">
         <v>0</v>
@@ -3731,7 +3697,7 @@
         <v>0</v>
       </c>
       <c r="P63" s="55">
-        <v>14.290217037955378</v>
+        <v>14.37364116419994</v>
       </c>
       <c r="Q63" s="3"/>
     </row>
@@ -3790,7 +3756,7 @@
   <dimension ref="B2:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3917,7 +3883,7 @@
         <v>126906</v>
       </c>
       <c r="I7" s="34">
-        <v>0</v>
+        <v>141433</v>
       </c>
       <c r="J7" s="34">
         <v>0</v>
@@ -3938,7 +3904,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="35">
-        <v>588693</v>
+        <v>730126</v>
       </c>
       <c r="Q7" s="2"/>
     </row>
@@ -3963,7 +3929,7 @@
         <v>62078</v>
       </c>
       <c r="I8" s="15">
-        <v>0</v>
+        <v>79656</v>
       </c>
       <c r="J8" s="15">
         <v>0</v>
@@ -3984,7 +3950,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="15">
-        <v>313279</v>
+        <v>392935</v>
       </c>
       <c r="Q8" s="3"/>
     </row>
@@ -4009,7 +3975,7 @@
         <v>62149</v>
       </c>
       <c r="I9" s="15">
-        <v>0</v>
+        <v>59262</v>
       </c>
       <c r="J9" s="15">
         <v>0</v>
@@ -4030,7 +3996,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="15">
-        <v>263800</v>
+        <v>323062</v>
       </c>
       <c r="Q9" s="3"/>
     </row>
@@ -4055,7 +4021,7 @@
         <v>2679</v>
       </c>
       <c r="I10" s="33">
-        <v>0</v>
+        <v>2515</v>
       </c>
       <c r="J10" s="33">
         <v>0</v>
@@ -4076,7 +4042,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="33">
-        <v>11614</v>
+        <v>14129</v>
       </c>
       <c r="Q10" s="3"/>
     </row>
@@ -4205,7 +4171,7 @@
         <v>48.916520889477248</v>
       </c>
       <c r="I19" s="61">
-        <v>0</v>
+        <v>56.320660666181155</v>
       </c>
       <c r="J19" s="61">
         <v>0</v>
@@ -4226,7 +4192,7 @@
         <v>0</v>
       </c>
       <c r="P19" s="61">
-        <v>53.216022612804977</v>
+        <v>53.81742329406157</v>
       </c>
     </row>
     <row r="20" spans="2:16" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -4250,7 +4216,7 @@
         <v>48.972467810820611</v>
       </c>
       <c r="I20" s="29">
-        <v>0</v>
+        <v>41.901112187396151</v>
       </c>
       <c r="J20" s="29">
         <v>0</v>
@@ -4271,7 +4237,7 @@
         <v>0</v>
       </c>
       <c r="P20" s="29">
-        <v>44.81113245783456</v>
+        <v>44.247431265288455</v>
       </c>
     </row>
     <row r="21" spans="2:16" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -4295,7 +4261,7 @@
         <v>2.1110112997021417</v>
       </c>
       <c r="I21" s="62">
-        <v>0</v>
+        <v>1.7782271464226878</v>
       </c>
       <c r="J21" s="62">
         <v>0</v>
@@ -4316,7 +4282,7 @@
         <v>0</v>
       </c>
       <c r="P21" s="62">
-        <v>1.9728449293604646</v>
+        <v>1.93514544064997</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -4340,8 +4306,8 @@
   </sheetPr>
   <dimension ref="B2:R49"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A37" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4488,7 +4454,7 @@
         <v>5052</v>
       </c>
       <c r="I7" s="101">
-        <v>0</v>
+        <v>4710</v>
       </c>
       <c r="J7" s="101">
         <v>0</v>
@@ -4509,7 +4475,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="101">
-        <v>19742</v>
+        <v>24452</v>
       </c>
     </row>
     <row r="8" spans="2:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4533,7 +4499,7 @@
         <v>610</v>
       </c>
       <c r="I8" s="15">
-        <v>0</v>
+        <v>618</v>
       </c>
       <c r="J8" s="15">
         <v>0</v>
@@ -4554,7 +4520,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="15">
-        <v>3142</v>
+        <v>3760</v>
       </c>
     </row>
     <row r="9" spans="2:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4578,7 +4544,7 @@
         <v>5821</v>
       </c>
       <c r="I9" s="15">
-        <v>0</v>
+        <v>5607</v>
       </c>
       <c r="J9" s="15">
         <v>0</v>
@@ -4599,7 +4565,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="15">
-        <v>22863</v>
+        <v>28470</v>
       </c>
     </row>
     <row r="10" spans="2:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4623,7 +4589,7 @@
         <v>136097</v>
       </c>
       <c r="I10" s="15">
-        <v>0</v>
+        <v>151901</v>
       </c>
       <c r="J10" s="15">
         <v>0</v>
@@ -4644,7 +4610,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="42">
-        <v>625199</v>
+        <v>777100</v>
       </c>
     </row>
     <row r="11" spans="2:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4668,7 +4634,7 @@
         <v>18801</v>
       </c>
       <c r="I11" s="41">
-        <v>0</v>
+        <v>17029</v>
       </c>
       <c r="J11" s="41">
         <v>0</v>
@@ -4689,7 +4655,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="33">
-        <v>83872</v>
+        <v>100901</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
@@ -4848,7 +4814,7 @@
         <v>3.0364043971366921</v>
       </c>
       <c r="I21" s="61">
-        <v>0</v>
+        <v>2.6186306396464012</v>
       </c>
       <c r="J21" s="61">
         <v>0</v>
@@ -4869,7 +4835,7 @@
         <v>0</v>
       </c>
       <c r="P21" s="61">
-        <v>2.6154649200204552</v>
+        <v>2.6160741128275578</v>
       </c>
     </row>
     <row r="22" spans="2:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4893,7 +4859,7 @@
         <v>0.36662840107945016</v>
       </c>
       <c r="I22" s="29">
-        <v>0</v>
+        <v>0.34359102660328578</v>
       </c>
       <c r="J22" s="29">
         <v>0</v>
@@ -4914,7 +4880,7 @@
         <v>0</v>
       </c>
       <c r="P22" s="29">
-        <v>0.41625928369487747</v>
+        <v>0.40227542386028203</v>
       </c>
     </row>
     <row r="23" spans="2:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4938,7 +4904,7 @@
         <v>3.498596594563081</v>
       </c>
       <c r="I23" s="29">
-        <v>0</v>
+        <v>3.1173380035026272</v>
       </c>
       <c r="J23" s="29">
         <v>0</v>
@@ -4959,7 +4925,7 @@
         <v>0</v>
       </c>
       <c r="P23" s="29">
-        <v>3.0289420761031134</v>
+        <v>3.0459524780059124</v>
       </c>
     </row>
     <row r="24" spans="2:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4983,7 +4949,7 @@
         <v>81.798402461819563</v>
       </c>
       <c r="I24" s="29">
-        <v>0</v>
+        <v>84.452784032468799</v>
       </c>
       <c r="J24" s="29">
         <v>0</v>
@@ -5004,7 +4970,7 @@
         <v>0</v>
       </c>
       <c r="P24" s="29">
-        <v>82.827781001512946</v>
+        <v>83.140487202613073</v>
       </c>
     </row>
     <row r="25" spans="2:16" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5028,7 +4994,7 @@
         <v>11.299968145401218</v>
       </c>
       <c r="I25" s="62">
-        <v>0</v>
+        <v>9.4676562977788894</v>
       </c>
       <c r="J25" s="62">
         <v>0</v>
@@ -5049,7 +5015,7 @@
         <v>0</v>
       </c>
       <c r="P25" s="62">
-        <v>11.111552718668607</v>
+        <v>10.79521078269317</v>
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
@@ -5191,7 +5157,7 @@
         <v>22</v>
       </c>
       <c r="I35" s="40">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J35" s="40">
         <v>0</v>
@@ -5212,7 +5178,7 @@
         <v>0</v>
       </c>
       <c r="P35" s="42">
-        <v>205</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5236,7 +5202,7 @@
         <v>2</v>
       </c>
       <c r="I36" s="40">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J36" s="40">
         <v>0</v>
@@ -5257,7 +5223,7 @@
         <v>0</v>
       </c>
       <c r="P36" s="42">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5281,7 +5247,7 @@
         <v>10119</v>
       </c>
       <c r="I37" s="41">
-        <v>0</v>
+        <v>9643</v>
       </c>
       <c r="J37" s="41">
         <v>0</v>
@@ -5302,7 +5268,7 @@
         <v>0</v>
       </c>
       <c r="P37" s="33">
-        <v>53962</v>
+        <v>63605</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
@@ -5446,7 +5412,7 @@
         <v>0.21689835354431627</v>
       </c>
       <c r="I47" s="40">
-        <v>0</v>
+        <v>0.14488254165373071</v>
       </c>
       <c r="J47" s="40">
         <v>0</v>
@@ -5467,7 +5433,7 @@
         <v>0</v>
       </c>
       <c r="P47" s="42">
-        <v>0.37815203556473781</v>
+        <v>0.34286251056768013</v>
       </c>
     </row>
     <row r="48" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5491,7 +5457,7 @@
         <v>1.9718032140392389E-2</v>
       </c>
       <c r="I48" s="40">
-        <v>0</v>
+        <v>6.2092517851598882E-2</v>
       </c>
       <c r="J48" s="40">
         <v>0</v>
@@ -5512,7 +5478,7 @@
         <v>0</v>
       </c>
       <c r="P48" s="42">
-        <v>8.1164339340724201E-2</v>
+        <v>7.8279112001753456E-2</v>
       </c>
     </row>
     <row r="49" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5536,7 +5502,7 @@
         <v>99.763383614315288</v>
       </c>
       <c r="I49" s="41">
-        <v>0</v>
+        <v>99.793024940494661</v>
       </c>
       <c r="J49" s="41">
         <v>0</v>
@@ -5557,7 +5523,7 @@
         <v>0</v>
       </c>
       <c r="P49" s="33">
-        <v>99.540683625094545</v>
+        <v>99.578858377430564</v>
       </c>
     </row>
   </sheetData>
@@ -5580,7 +5546,7 @@
   <dimension ref="B2:Q146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5719,7 +5685,7 @@
         <v>176524</v>
       </c>
       <c r="J7" s="67">
-        <v>0</v>
+        <v>189528</v>
       </c>
       <c r="K7" s="67">
         <v>0</v>
@@ -5740,7 +5706,7 @@
         <v>0</v>
       </c>
       <c r="Q7" s="68">
-        <v>809029</v>
+        <v>998557</v>
       </c>
     </row>
     <row r="8" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5765,7 +5731,7 @@
         <v>127508</v>
       </c>
       <c r="J8" s="97">
-        <v>0</v>
+        <v>142037</v>
       </c>
       <c r="K8" s="97">
         <v>0</v>
@@ -5786,7 +5752,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="97">
-        <v>591678</v>
+        <v>733715</v>
       </c>
     </row>
     <row r="9" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5799,19 +5765,19 @@
         <v>102313</v>
       </c>
       <c r="F9" s="102">
-        <v>94515</v>
+        <v>94516</v>
       </c>
       <c r="G9" s="102">
-        <v>144005</v>
+        <v>144011</v>
       </c>
       <c r="H9" s="102">
-        <v>116600</v>
+        <v>116606</v>
       </c>
       <c r="I9" s="102">
-        <v>124444</v>
+        <v>124461</v>
       </c>
       <c r="J9" s="102">
-        <v>0</v>
+        <v>139255</v>
       </c>
       <c r="K9" s="102">
         <v>0</v>
@@ -5832,7 +5798,7 @@
         <v>0</v>
       </c>
       <c r="Q9" s="102">
-        <v>581877</v>
+        <v>721162</v>
       </c>
     </row>
     <row r="10" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5857,7 +5823,7 @@
         <v>461</v>
       </c>
       <c r="J10" s="15">
-        <v>0</v>
+        <v>606</v>
       </c>
       <c r="K10" s="15">
         <v>0</v>
@@ -5878,7 +5844,7 @@
         <v>0</v>
       </c>
       <c r="Q10" s="15">
-        <v>2280</v>
+        <v>2886</v>
       </c>
     </row>
     <row r="11" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5891,19 +5857,19 @@
         <v>905</v>
       </c>
       <c r="F11" s="15">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="G11" s="15">
-        <v>1517</v>
+        <v>1523</v>
       </c>
       <c r="H11" s="15">
-        <v>1155</v>
+        <v>1161</v>
       </c>
       <c r="I11" s="15">
-        <v>1410</v>
+        <v>1427</v>
       </c>
       <c r="J11" s="15">
-        <v>0</v>
+        <v>1206</v>
       </c>
       <c r="K11" s="15">
         <v>0</v>
@@ -5924,7 +5890,7 @@
         <v>0</v>
       </c>
       <c r="Q11" s="15">
-        <v>5836</v>
+        <v>7072</v>
       </c>
     </row>
     <row r="12" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5949,7 +5915,7 @@
         <v>1312</v>
       </c>
       <c r="J12" s="15">
-        <v>0</v>
+        <v>1114</v>
       </c>
       <c r="K12" s="15">
         <v>0</v>
@@ -5970,7 +5936,7 @@
         <v>0</v>
       </c>
       <c r="Q12" s="15">
-        <v>5257</v>
+        <v>6371</v>
       </c>
     </row>
     <row r="13" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5983,19 +5949,19 @@
         <v>123</v>
       </c>
       <c r="F13" s="15">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G13" s="15">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="H13" s="15">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="I13" s="15">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="J13" s="15">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="K13" s="15">
         <v>0</v>
@@ -6016,7 +5982,7 @@
         <v>0</v>
       </c>
       <c r="Q13" s="15">
-        <v>579</v>
+        <v>701</v>
       </c>
     </row>
     <row r="14" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6041,7 +6007,7 @@
         <v>2004</v>
       </c>
       <c r="J14" s="15">
-        <v>0</v>
+        <v>2836</v>
       </c>
       <c r="K14" s="15">
         <v>0</v>
@@ -6062,7 +6028,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="15">
-        <v>8063</v>
+        <v>10899</v>
       </c>
     </row>
     <row r="15" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6087,7 +6053,7 @@
         <v>1966</v>
       </c>
       <c r="J15" s="15">
-        <v>0</v>
+        <v>2779</v>
       </c>
       <c r="K15" s="15">
         <v>0</v>
@@ -6108,7 +6074,7 @@
         <v>0</v>
       </c>
       <c r="Q15" s="15">
-        <v>7831</v>
+        <v>10610</v>
       </c>
     </row>
     <row r="16" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6133,7 +6099,7 @@
         <v>22</v>
       </c>
       <c r="J16" s="15">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K16" s="15">
         <v>0</v>
@@ -6154,7 +6120,7 @@
         <v>0</v>
       </c>
       <c r="Q16" s="15">
-        <v>104</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6179,7 +6145,7 @@
         <v>16</v>
       </c>
       <c r="J17" s="15">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="K17" s="15">
         <v>0</v>
@@ -6200,7 +6166,7 @@
         <v>0</v>
       </c>
       <c r="Q17" s="15">
-        <v>128</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6225,7 +6191,7 @@
         <v>30108</v>
       </c>
       <c r="J18" s="15">
-        <v>0</v>
+        <v>36197</v>
       </c>
       <c r="K18" s="15">
         <v>0</v>
@@ -6246,7 +6212,7 @@
         <v>0</v>
       </c>
       <c r="Q18" s="15">
-        <v>147757</v>
+        <v>183954</v>
       </c>
     </row>
     <row r="19" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6271,7 +6237,7 @@
         <v>2</v>
       </c>
       <c r="J19" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K19" s="15">
         <v>0</v>
@@ -6292,7 +6258,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="15">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6317,7 +6283,7 @@
         <v>6</v>
       </c>
       <c r="J20" s="15">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K20" s="15">
         <v>0</v>
@@ -6338,7 +6304,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="15">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6363,7 +6329,7 @@
         <v>18295</v>
       </c>
       <c r="J21" s="15">
-        <v>0</v>
+        <v>26402</v>
       </c>
       <c r="K21" s="15">
         <v>0</v>
@@ -6384,7 +6350,7 @@
         <v>0</v>
       </c>
       <c r="Q21" s="15">
-        <v>94181</v>
+        <v>120583</v>
       </c>
     </row>
     <row r="22" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6409,7 +6375,7 @@
         <v>11805</v>
       </c>
       <c r="J22" s="15">
-        <v>0</v>
+        <v>9782</v>
       </c>
       <c r="K22" s="15">
         <v>0</v>
@@ -6430,7 +6396,7 @@
         <v>0</v>
       </c>
       <c r="Q22" s="15">
-        <v>53531</v>
+        <v>63313</v>
       </c>
     </row>
     <row r="23" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6455,7 +6421,7 @@
         <v>342</v>
       </c>
       <c r="J23" s="15">
-        <v>0</v>
+        <v>262</v>
       </c>
       <c r="K23" s="15">
         <v>0</v>
@@ -6476,7 +6442,7 @@
         <v>0</v>
       </c>
       <c r="Q23" s="15">
-        <v>1079</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="24" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6501,7 +6467,7 @@
         <v>20250</v>
       </c>
       <c r="J24" s="15">
-        <v>0</v>
+        <v>21737</v>
       </c>
       <c r="K24" s="15">
         <v>0</v>
@@ -6522,7 +6488,7 @@
         <v>0</v>
       </c>
       <c r="Q24" s="15">
-        <v>99385</v>
+        <v>121122</v>
       </c>
     </row>
     <row r="25" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6547,7 +6513,7 @@
         <v>6708</v>
       </c>
       <c r="J25" s="15">
-        <v>0</v>
+        <v>6665</v>
       </c>
       <c r="K25" s="15">
         <v>0</v>
@@ -6568,7 +6534,7 @@
         <v>0</v>
       </c>
       <c r="Q25" s="15">
-        <v>27446</v>
+        <v>34111</v>
       </c>
     </row>
     <row r="26" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6593,7 +6559,7 @@
         <v>401</v>
       </c>
       <c r="J26" s="15">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="K26" s="15">
         <v>0</v>
@@ -6614,7 +6580,7 @@
         <v>0</v>
       </c>
       <c r="Q26" s="15">
-        <v>2246</v>
+        <v>2846</v>
       </c>
     </row>
     <row r="27" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6639,7 +6605,7 @@
         <v>332</v>
       </c>
       <c r="J27" s="15">
-        <v>0</v>
+        <v>508</v>
       </c>
       <c r="K27" s="15">
         <v>0</v>
@@ -6660,7 +6626,7 @@
         <v>0</v>
       </c>
       <c r="Q27" s="15">
-        <v>1777</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="28" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6685,7 +6651,7 @@
         <v>69</v>
       </c>
       <c r="J28" s="15">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="K28" s="15">
         <v>0</v>
@@ -6706,7 +6672,7 @@
         <v>0</v>
       </c>
       <c r="Q28" s="15">
-        <v>469</v>
+        <v>561</v>
       </c>
     </row>
     <row r="29" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6731,7 +6697,7 @@
         <v>10897</v>
       </c>
       <c r="J29" s="15">
-        <v>0</v>
+        <v>12412</v>
       </c>
       <c r="K29" s="15">
         <v>0</v>
@@ -6752,7 +6718,7 @@
         <v>0</v>
       </c>
       <c r="Q29" s="15">
-        <v>61043</v>
+        <v>73455</v>
       </c>
     </row>
     <row r="30" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6777,7 +6743,7 @@
         <v>478</v>
       </c>
       <c r="J30" s="15">
-        <v>0</v>
+        <v>496</v>
       </c>
       <c r="K30" s="15">
         <v>0</v>
@@ -6798,7 +6764,7 @@
         <v>0</v>
       </c>
       <c r="Q30" s="15">
-        <v>1976</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="31" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6823,7 +6789,7 @@
         <v>27</v>
       </c>
       <c r="J31" s="15">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="K31" s="15">
         <v>0</v>
@@ -6844,7 +6810,7 @@
         <v>0</v>
       </c>
       <c r="Q31" s="15">
-        <v>180</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6869,7 +6835,7 @@
         <v>451</v>
       </c>
       <c r="J32" s="15">
-        <v>0</v>
+        <v>467</v>
       </c>
       <c r="K32" s="15">
         <v>0</v>
@@ -6890,7 +6856,7 @@
         <v>0</v>
       </c>
       <c r="Q32" s="15">
-        <v>1796</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="33" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6915,7 +6881,7 @@
         <v>336</v>
       </c>
       <c r="J33" s="15">
-        <v>0</v>
+        <v>275</v>
       </c>
       <c r="K33" s="15">
         <v>0</v>
@@ -6936,7 +6902,7 @@
         <v>0</v>
       </c>
       <c r="Q33" s="15">
-        <v>2066</v>
+        <v>2341</v>
       </c>
     </row>
     <row r="34" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -6961,7 +6927,7 @@
         <v>5531</v>
       </c>
       <c r="J34" s="15">
-        <v>0</v>
+        <v>4781</v>
       </c>
       <c r="K34" s="15">
         <v>0</v>
@@ -6982,7 +6948,7 @@
         <v>0</v>
       </c>
       <c r="Q34" s="15">
-        <v>22974</v>
+        <v>27755</v>
       </c>
     </row>
     <row r="35" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7007,7 +6973,7 @@
         <v>4500</v>
       </c>
       <c r="J35" s="15">
-        <v>0</v>
+        <v>6001</v>
       </c>
       <c r="K35" s="15">
         <v>0</v>
@@ -7028,7 +6994,7 @@
         <v>0</v>
       </c>
       <c r="Q35" s="15">
-        <v>19908</v>
+        <v>25909</v>
       </c>
     </row>
     <row r="36" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7053,7 +7019,7 @@
         <v>2653</v>
       </c>
       <c r="J36" s="15">
-        <v>0</v>
+        <v>2928</v>
       </c>
       <c r="K36" s="15">
         <v>0</v>
@@ -7074,7 +7040,7 @@
         <v>0</v>
       </c>
       <c r="Q36" s="15">
-        <v>9806</v>
+        <v>12734</v>
       </c>
     </row>
     <row r="37" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7099,7 +7065,7 @@
         <v>1847</v>
       </c>
       <c r="J37" s="15">
-        <v>0</v>
+        <v>3073</v>
       </c>
       <c r="K37" s="15">
         <v>0</v>
@@ -7120,7 +7086,7 @@
         <v>0</v>
       </c>
       <c r="Q37" s="15">
-        <v>10102</v>
+        <v>13175</v>
       </c>
     </row>
     <row r="38" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7145,7 +7111,7 @@
         <v>5761</v>
       </c>
       <c r="J38" s="15">
-        <v>0</v>
+        <v>8917</v>
       </c>
       <c r="K38" s="15">
         <v>0</v>
@@ -7166,7 +7132,7 @@
         <v>0</v>
       </c>
       <c r="Q38" s="15">
-        <v>33617</v>
+        <v>42534</v>
       </c>
     </row>
     <row r="39" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7191,7 +7157,7 @@
         <v>12559</v>
       </c>
       <c r="J39" s="15">
-        <v>0</v>
+        <v>11761</v>
       </c>
       <c r="K39" s="15">
         <v>0</v>
@@ -7212,7 +7178,7 @@
         <v>0</v>
       </c>
       <c r="Q39" s="15">
-        <v>55214</v>
+        <v>66975</v>
       </c>
     </row>
     <row r="40" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7237,7 +7203,7 @@
         <v>12458</v>
       </c>
       <c r="J40" s="15">
-        <v>0</v>
+        <v>11660</v>
       </c>
       <c r="K40" s="15">
         <v>0</v>
@@ -7258,7 +7224,7 @@
         <v>0</v>
       </c>
       <c r="Q40" s="15">
-        <v>54983</v>
+        <v>66643</v>
       </c>
     </row>
     <row r="41" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7283,7 +7249,7 @@
         <v>101</v>
       </c>
       <c r="J41" s="15">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="K41" s="15">
         <v>0</v>
@@ -7304,7 +7270,7 @@
         <v>0</v>
       </c>
       <c r="Q41" s="15">
-        <v>231</v>
+        <v>332</v>
       </c>
     </row>
     <row r="42" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7329,7 +7295,7 @@
         <v>22698</v>
       </c>
       <c r="J42" s="15">
-        <v>0</v>
+        <v>24503</v>
       </c>
       <c r="K42" s="15">
         <v>0</v>
@@ -7350,7 +7316,7 @@
         <v>0</v>
       </c>
       <c r="Q42" s="15">
-        <v>90987</v>
+        <v>115490</v>
       </c>
     </row>
     <row r="43" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7363,19 +7329,19 @@
         <v>1573</v>
       </c>
       <c r="F43" s="43">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="G43" s="43">
-        <v>2239</v>
+        <v>2233</v>
       </c>
       <c r="H43" s="43">
-        <v>1577</v>
+        <v>1571</v>
       </c>
       <c r="I43" s="43">
-        <v>3064</v>
+        <v>3047</v>
       </c>
       <c r="J43" s="43">
-        <v>0</v>
+        <v>2782</v>
       </c>
       <c r="K43" s="43">
         <v>0</v>
@@ -7396,7 +7362,7 @@
         <v>0</v>
       </c>
       <c r="Q43" s="43">
-        <v>9801</v>
+        <v>12553</v>
       </c>
     </row>
     <row r="44" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7421,7 +7387,7 @@
         <v>38873</v>
       </c>
       <c r="J44" s="93">
-        <v>0</v>
+        <v>37833</v>
       </c>
       <c r="K44" s="93">
         <v>0</v>
@@ -7442,7 +7408,7 @@
         <v>0</v>
       </c>
       <c r="Q44" s="93">
-        <v>163140</v>
+        <v>200973</v>
       </c>
     </row>
     <row r="45" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7452,7 +7418,7 @@
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="21">
-        <v>26465</v>
+        <v>26464</v>
       </c>
       <c r="F45" s="21">
         <v>23742</v>
@@ -7464,10 +7430,10 @@
         <v>32997</v>
       </c>
       <c r="I45" s="21">
-        <v>38523</v>
+        <v>38554</v>
       </c>
       <c r="J45" s="21">
-        <v>0</v>
+        <v>37612</v>
       </c>
       <c r="K45" s="21">
         <v>0</v>
@@ -7488,7 +7454,7 @@
         <v>0</v>
       </c>
       <c r="Q45" s="21">
-        <v>161414</v>
+        <v>199056</v>
       </c>
     </row>
     <row r="46" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7513,7 +7479,7 @@
         <v>11</v>
       </c>
       <c r="J46" s="15">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="K46" s="15">
         <v>0</v>
@@ -7534,7 +7500,7 @@
         <v>0</v>
       </c>
       <c r="Q46" s="15">
-        <v>17</v>
+        <v>49</v>
       </c>
     </row>
     <row r="47" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7556,10 +7522,10 @@
         <v>13797</v>
       </c>
       <c r="I47" s="15">
-        <v>16427</v>
+        <v>16458</v>
       </c>
       <c r="J47" s="15">
-        <v>0</v>
+        <v>16421</v>
       </c>
       <c r="K47" s="15">
         <v>0</v>
@@ -7580,7 +7546,7 @@
         <v>0</v>
       </c>
       <c r="Q47" s="15">
-        <v>71791</v>
+        <v>88243</v>
       </c>
     </row>
     <row r="48" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7602,10 +7568,10 @@
         <v>210</v>
       </c>
       <c r="I48" s="15">
-        <v>274</v>
+        <v>305</v>
       </c>
       <c r="J48" s="15">
-        <v>0</v>
+        <v>412</v>
       </c>
       <c r="K48" s="15">
         <v>0</v>
@@ -7626,7 +7592,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="15">
-        <v>1410</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="49" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7651,7 +7617,7 @@
         <v>16153</v>
       </c>
       <c r="J49" s="15">
-        <v>0</v>
+        <v>16009</v>
       </c>
       <c r="K49" s="15">
         <v>0</v>
@@ -7672,7 +7638,7 @@
         <v>0</v>
       </c>
       <c r="Q49" s="15">
-        <v>70381</v>
+        <v>86390</v>
       </c>
     </row>
     <row r="50" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7697,7 +7663,7 @@
         <v>2123</v>
       </c>
       <c r="J50" s="15">
-        <v>0</v>
+        <v>1879</v>
       </c>
       <c r="K50" s="15">
         <v>0</v>
@@ -7718,7 +7684,7 @@
         <v>0</v>
       </c>
       <c r="Q50" s="15">
-        <v>9083</v>
+        <v>10962</v>
       </c>
     </row>
     <row r="51" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7728,7 +7694,7 @@
         <v>89</v>
       </c>
       <c r="E51" s="15">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="F51" s="15">
         <v>1865</v>
@@ -7743,7 +7709,7 @@
         <v>5973</v>
       </c>
       <c r="J51" s="15">
-        <v>0</v>
+        <v>5402</v>
       </c>
       <c r="K51" s="15">
         <v>0</v>
@@ -7764,7 +7730,7 @@
         <v>0</v>
       </c>
       <c r="Q51" s="15">
-        <v>22521</v>
+        <v>27922</v>
       </c>
     </row>
     <row r="52" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7789,7 +7755,7 @@
         <v>937</v>
       </c>
       <c r="J52" s="15">
-        <v>0</v>
+        <v>965</v>
       </c>
       <c r="K52" s="15">
         <v>0</v>
@@ -7810,7 +7776,7 @@
         <v>0</v>
       </c>
       <c r="Q52" s="15">
-        <v>4269</v>
+        <v>5234</v>
       </c>
     </row>
     <row r="53" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7835,7 +7801,7 @@
         <v>260</v>
       </c>
       <c r="J53" s="15">
-        <v>0</v>
+        <v>278</v>
       </c>
       <c r="K53" s="15">
         <v>0</v>
@@ -7856,7 +7822,7 @@
         <v>0</v>
       </c>
       <c r="Q53" s="15">
-        <v>922</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="54" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7881,7 +7847,7 @@
         <v>1</v>
       </c>
       <c r="J54" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K54" s="15">
         <v>0</v>
@@ -7902,7 +7868,7 @@
         <v>0</v>
       </c>
       <c r="Q54" s="15">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7927,7 +7893,7 @@
         <v>158</v>
       </c>
       <c r="J55" s="15">
-        <v>0</v>
+        <v>149</v>
       </c>
       <c r="K55" s="15">
         <v>0</v>
@@ -7948,7 +7914,7 @@
         <v>0</v>
       </c>
       <c r="Q55" s="15">
-        <v>778</v>
+        <v>927</v>
       </c>
     </row>
     <row r="56" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -7973,7 +7939,7 @@
         <v>536</v>
       </c>
       <c r="J56" s="15">
-        <v>0</v>
+        <v>502</v>
       </c>
       <c r="K56" s="15">
         <v>0</v>
@@ -7994,7 +7960,7 @@
         <v>0</v>
       </c>
       <c r="Q56" s="15">
-        <v>2771</v>
+        <v>3273</v>
       </c>
     </row>
     <row r="57" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8019,7 +7985,7 @@
         <v>810</v>
       </c>
       <c r="J57" s="15">
-        <v>0</v>
+        <v>955</v>
       </c>
       <c r="K57" s="15">
         <v>0</v>
@@ -8040,7 +8006,7 @@
         <v>0</v>
       </c>
       <c r="Q57" s="15">
-        <v>2923</v>
+        <v>3878</v>
       </c>
     </row>
     <row r="58" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8065,7 +8031,7 @@
         <v>410</v>
       </c>
       <c r="J58" s="15">
-        <v>0</v>
+        <v>374</v>
       </c>
       <c r="K58" s="15">
         <v>0</v>
@@ -8086,7 +8052,7 @@
         <v>0</v>
       </c>
       <c r="Q58" s="15">
-        <v>2081</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="59" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8111,7 +8077,7 @@
         <v>276</v>
       </c>
       <c r="J59" s="15">
-        <v>0</v>
+        <v>277</v>
       </c>
       <c r="K59" s="15">
         <v>0</v>
@@ -8132,7 +8098,7 @@
         <v>0</v>
       </c>
       <c r="Q59" s="15">
-        <v>1115</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="60" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8157,7 +8123,7 @@
         <v>134</v>
       </c>
       <c r="J60" s="15">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="K60" s="15">
         <v>0</v>
@@ -8178,7 +8144,7 @@
         <v>0</v>
       </c>
       <c r="Q60" s="15">
-        <v>966</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="61" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8203,7 +8169,7 @@
         <v>2197</v>
       </c>
       <c r="J61" s="15">
-        <v>0</v>
+        <v>1653</v>
       </c>
       <c r="K61" s="15">
         <v>0</v>
@@ -8224,7 +8190,7 @@
         <v>0</v>
       </c>
       <c r="Q61" s="15">
-        <v>8805</v>
+        <v>10458</v>
       </c>
     </row>
     <row r="62" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8249,7 +8215,7 @@
         <v>3990</v>
       </c>
       <c r="J62" s="15">
-        <v>0</v>
+        <v>3732</v>
       </c>
       <c r="K62" s="15">
         <v>0</v>
@@ -8270,7 +8236,7 @@
         <v>0</v>
       </c>
       <c r="Q62" s="15">
-        <v>17811</v>
+        <v>21543</v>
       </c>
     </row>
     <row r="63" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8295,7 +8261,7 @@
         <v>4690</v>
       </c>
       <c r="J63" s="15">
-        <v>0</v>
+        <v>5269</v>
       </c>
       <c r="K63" s="15">
         <v>0</v>
@@ -8316,7 +8282,7 @@
         <v>0</v>
       </c>
       <c r="Q63" s="15">
-        <v>17632</v>
+        <v>22901</v>
       </c>
     </row>
     <row r="64" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8326,7 +8292,7 @@
       </c>
       <c r="D64" s="95"/>
       <c r="E64" s="43">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="F64" s="43">
         <v>301</v>
@@ -8338,10 +8304,10 @@
         <v>323</v>
       </c>
       <c r="I64" s="43">
-        <v>350</v>
+        <v>319</v>
       </c>
       <c r="J64" s="43">
-        <v>0</v>
+        <v>221</v>
       </c>
       <c r="K64" s="43">
         <v>0</v>
@@ -8362,7 +8328,7 @@
         <v>0</v>
       </c>
       <c r="Q64" s="33">
-        <v>1726</v>
+        <v>1917</v>
       </c>
     </row>
     <row r="65" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8387,7 +8353,7 @@
         <v>8223</v>
       </c>
       <c r="J65" s="97">
-        <v>0</v>
+        <v>7884</v>
       </c>
       <c r="K65" s="97">
         <v>0</v>
@@ -8408,7 +8374,7 @@
         <v>0</v>
       </c>
       <c r="Q65" s="97">
-        <v>44663</v>
+        <v>52547</v>
       </c>
     </row>
     <row r="66" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8433,7 +8399,7 @@
         <v>773</v>
       </c>
       <c r="J66" s="94">
-        <v>0</v>
+        <v>512</v>
       </c>
       <c r="K66" s="94">
         <v>0</v>
@@ -8454,7 +8420,7 @@
         <v>0</v>
       </c>
       <c r="Q66" s="94">
-        <v>4059</v>
+        <v>4571</v>
       </c>
     </row>
     <row r="67" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8479,7 +8445,7 @@
         <v>772</v>
       </c>
       <c r="J67" s="21">
-        <v>0</v>
+        <v>507</v>
       </c>
       <c r="K67" s="21">
         <v>0</v>
@@ -8500,7 +8466,7 @@
         <v>0</v>
       </c>
       <c r="Q67" s="21">
-        <v>4046</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="68" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8525,7 +8491,7 @@
         <v>0</v>
       </c>
       <c r="J68" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K68" s="21">
         <v>0</v>
@@ -8546,7 +8512,7 @@
         <v>0</v>
       </c>
       <c r="Q68" s="15">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8571,7 +8537,7 @@
         <v>433</v>
       </c>
       <c r="J69" s="21">
-        <v>0</v>
+        <v>209</v>
       </c>
       <c r="K69" s="21">
         <v>0</v>
@@ -8592,7 +8558,7 @@
         <v>0</v>
       </c>
       <c r="Q69" s="15">
-        <v>2573</v>
+        <v>2782</v>
       </c>
     </row>
     <row r="70" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8617,7 +8583,7 @@
         <v>3</v>
       </c>
       <c r="J70" s="21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K70" s="21">
         <v>0</v>
@@ -8638,7 +8604,7 @@
         <v>0</v>
       </c>
       <c r="Q70" s="15">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8663,7 +8629,7 @@
         <v>65</v>
       </c>
       <c r="J71" s="21">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="K71" s="21">
         <v>0</v>
@@ -8684,7 +8650,7 @@
         <v>0</v>
       </c>
       <c r="Q71" s="15">
-        <v>294</v>
+        <v>328</v>
       </c>
     </row>
     <row r="72" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8709,7 +8675,7 @@
         <v>56</v>
       </c>
       <c r="J72" s="15">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="K72" s="15">
         <v>0</v>
@@ -8730,7 +8696,7 @@
         <v>0</v>
       </c>
       <c r="Q72" s="15">
-        <v>157</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8755,7 +8721,7 @@
         <v>209</v>
       </c>
       <c r="J73" s="15">
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="K73" s="15">
         <v>0</v>
@@ -8776,7 +8742,7 @@
         <v>0</v>
       </c>
       <c r="Q73" s="15">
-        <v>984</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="74" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8801,7 +8767,7 @@
         <v>6</v>
       </c>
       <c r="J74" s="15">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="K74" s="15">
         <v>0</v>
@@ -8822,7 +8788,7 @@
         <v>0</v>
       </c>
       <c r="Q74" s="15">
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="75" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8847,7 +8813,7 @@
         <v>5</v>
       </c>
       <c r="J75" s="15">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K75" s="15">
         <v>0</v>
@@ -8868,7 +8834,7 @@
         <v>0</v>
       </c>
       <c r="Q75" s="15">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8893,7 +8859,7 @@
         <v>1</v>
       </c>
       <c r="J76" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K76" s="15">
         <v>0</v>
@@ -8914,7 +8880,7 @@
         <v>0</v>
       </c>
       <c r="Q76" s="15">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8939,7 +8905,7 @@
         <v>1</v>
       </c>
       <c r="J77" s="43">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K77" s="43">
         <v>0</v>
@@ -8960,7 +8926,7 @@
         <v>0</v>
       </c>
       <c r="Q77" s="43">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -8985,7 +8951,7 @@
         <v>698</v>
       </c>
       <c r="J78" s="94">
-        <v>0</v>
+        <v>658</v>
       </c>
       <c r="K78" s="94">
         <v>0</v>
@@ -9006,7 +8972,7 @@
         <v>0</v>
       </c>
       <c r="Q78" s="94">
-        <v>3887</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="79" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9031,7 +8997,7 @@
         <v>675</v>
       </c>
       <c r="J79" s="21">
-        <v>0</v>
+        <v>651</v>
       </c>
       <c r="K79" s="21">
         <v>0</v>
@@ -9052,7 +9018,7 @@
         <v>0</v>
       </c>
       <c r="Q79" s="21">
-        <v>3711</v>
+        <v>4362</v>
       </c>
     </row>
     <row r="80" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9077,7 +9043,7 @@
         <v>2</v>
       </c>
       <c r="J80" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K80" s="15">
         <v>0</v>
@@ -9098,7 +9064,7 @@
         <v>0</v>
       </c>
       <c r="Q80" s="15">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9123,7 +9089,7 @@
         <v>29</v>
       </c>
       <c r="J81" s="15">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K81" s="15">
         <v>0</v>
@@ -9144,7 +9110,7 @@
         <v>0</v>
       </c>
       <c r="Q81" s="15">
-        <v>150</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9169,7 +9135,7 @@
         <v>2</v>
       </c>
       <c r="J82" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K82" s="15">
         <v>0</v>
@@ -9190,7 +9156,7 @@
         <v>0</v>
       </c>
       <c r="Q82" s="15">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9215,7 +9181,7 @@
         <v>90</v>
       </c>
       <c r="J83" s="15">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="K83" s="15">
         <v>0</v>
@@ -9236,7 +9202,7 @@
         <v>0</v>
       </c>
       <c r="Q83" s="15">
-        <v>443</v>
+        <v>559</v>
       </c>
     </row>
     <row r="84" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9261,7 +9227,7 @@
         <v>235</v>
       </c>
       <c r="J84" s="15">
-        <v>0</v>
+        <v>218</v>
       </c>
       <c r="K84" s="15">
         <v>0</v>
@@ -9282,7 +9248,7 @@
         <v>0</v>
       </c>
       <c r="Q84" s="15">
-        <v>1010</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="85" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9307,7 +9273,7 @@
         <v>317</v>
       </c>
       <c r="J85" s="15">
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="K85" s="15">
         <v>0</v>
@@ -9328,7 +9294,7 @@
         <v>0</v>
       </c>
       <c r="Q85" s="15">
-        <v>2081</v>
+        <v>2370</v>
       </c>
     </row>
     <row r="86" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9353,7 +9319,7 @@
         <v>23</v>
       </c>
       <c r="J86" s="43">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K86" s="43">
         <v>0</v>
@@ -9374,7 +9340,7 @@
         <v>0</v>
       </c>
       <c r="Q86" s="43">
-        <v>176</v>
+        <v>183</v>
       </c>
     </row>
     <row r="87" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9399,7 +9365,7 @@
         <v>741</v>
       </c>
       <c r="J87" s="94">
-        <v>0</v>
+        <v>658</v>
       </c>
       <c r="K87" s="94">
         <v>0</v>
@@ -9420,7 +9386,7 @@
         <v>0</v>
       </c>
       <c r="Q87" s="94">
-        <v>3659</v>
+        <v>4317</v>
       </c>
     </row>
     <row r="88" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9445,7 +9411,7 @@
         <v>721</v>
       </c>
       <c r="J88" s="21">
-        <v>0</v>
+        <v>644</v>
       </c>
       <c r="K88" s="21">
         <v>0</v>
@@ -9466,7 +9432,7 @@
         <v>0</v>
       </c>
       <c r="Q88" s="21">
-        <v>3584</v>
+        <v>4228</v>
       </c>
     </row>
     <row r="89" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9491,7 +9457,7 @@
         <v>2</v>
       </c>
       <c r="J89" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K89" s="15">
         <v>0</v>
@@ -9512,7 +9478,7 @@
         <v>0</v>
       </c>
       <c r="Q89" s="15">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9629,7 +9595,7 @@
         <v>97</v>
       </c>
       <c r="J92" s="15">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="K92" s="15">
         <v>0</v>
@@ -9650,7 +9616,7 @@
         <v>0</v>
       </c>
       <c r="Q92" s="15">
-        <v>507</v>
+        <v>647</v>
       </c>
     </row>
     <row r="93" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9675,7 +9641,7 @@
         <v>525</v>
       </c>
       <c r="J93" s="15">
-        <v>0</v>
+        <v>433</v>
       </c>
       <c r="K93" s="15">
         <v>0</v>
@@ -9696,7 +9662,7 @@
         <v>0</v>
       </c>
       <c r="Q93" s="15">
-        <v>2475</v>
+        <v>2908</v>
       </c>
     </row>
     <row r="94" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9721,7 +9687,7 @@
         <v>97</v>
       </c>
       <c r="J94" s="15">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="K94" s="15">
         <v>0</v>
@@ -9742,7 +9708,7 @@
         <v>0</v>
       </c>
       <c r="Q94" s="15">
-        <v>596</v>
+        <v>666</v>
       </c>
     </row>
     <row r="95" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9767,7 +9733,7 @@
         <v>20</v>
       </c>
       <c r="J95" s="15">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K95" s="15">
         <v>0</v>
@@ -9788,7 +9754,7 @@
         <v>0</v>
       </c>
       <c r="Q95" s="43">
-        <v>75</v>
+        <v>89</v>
       </c>
     </row>
     <row r="96" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9813,7 +9779,7 @@
         <v>2284</v>
       </c>
       <c r="J96" s="94">
-        <v>0</v>
+        <v>2129</v>
       </c>
       <c r="K96" s="94">
         <v>0</v>
@@ -9834,7 +9800,7 @@
         <v>0</v>
       </c>
       <c r="Q96" s="94">
-        <v>12074</v>
+        <v>14203</v>
       </c>
     </row>
     <row r="97" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9859,7 +9825,7 @@
         <v>2283</v>
       </c>
       <c r="J97" s="21">
-        <v>0</v>
+        <v>2129</v>
       </c>
       <c r="K97" s="21">
         <v>0</v>
@@ -9880,7 +9846,7 @@
         <v>0</v>
       </c>
       <c r="Q97" s="21">
-        <v>12069</v>
+        <v>14198</v>
       </c>
     </row>
     <row r="98" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9905,7 +9871,7 @@
         <v>2</v>
       </c>
       <c r="J98" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K98" s="15">
         <v>0</v>
@@ -9926,7 +9892,7 @@
         <v>0</v>
       </c>
       <c r="Q98" s="15">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9951,7 +9917,7 @@
         <v>57</v>
       </c>
       <c r="J99" s="15">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="K99" s="15">
         <v>0</v>
@@ -9972,7 +9938,7 @@
         <v>0</v>
       </c>
       <c r="Q99" s="15">
-        <v>285</v>
+        <v>357</v>
       </c>
     </row>
     <row r="100" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9997,7 +9963,7 @@
         <v>0</v>
       </c>
       <c r="J100" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K100" s="15">
         <v>0</v>
@@ -10018,7 +9984,7 @@
         <v>0</v>
       </c>
       <c r="Q100" s="15">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10043,7 +10009,7 @@
         <v>401</v>
       </c>
       <c r="J101" s="15">
-        <v>0</v>
+        <v>457</v>
       </c>
       <c r="K101" s="15">
         <v>0</v>
@@ -10064,7 +10030,7 @@
         <v>0</v>
       </c>
       <c r="Q101" s="15">
-        <v>1802</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="102" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10089,7 +10055,7 @@
         <v>1048</v>
       </c>
       <c r="J102" s="15">
-        <v>0</v>
+        <v>892</v>
       </c>
       <c r="K102" s="15">
         <v>0</v>
@@ -10110,7 +10076,7 @@
         <v>0</v>
       </c>
       <c r="Q102" s="15">
-        <v>5318</v>
+        <v>6210</v>
       </c>
     </row>
     <row r="103" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10135,7 +10101,7 @@
         <v>472</v>
       </c>
       <c r="J103" s="15">
-        <v>0</v>
+        <v>397</v>
       </c>
       <c r="K103" s="15">
         <v>0</v>
@@ -10156,7 +10122,7 @@
         <v>0</v>
       </c>
       <c r="Q103" s="15">
-        <v>2855</v>
+        <v>3252</v>
       </c>
     </row>
     <row r="104" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10227,7 +10193,7 @@
         <v>303</v>
       </c>
       <c r="J105" s="15">
-        <v>0</v>
+        <v>309</v>
       </c>
       <c r="K105" s="15">
         <v>0</v>
@@ -10248,7 +10214,7 @@
         <v>0</v>
       </c>
       <c r="Q105" s="15">
-        <v>1799</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="106" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10319,7 +10285,7 @@
         <v>3727</v>
       </c>
       <c r="J107" s="94">
-        <v>0</v>
+        <v>3927</v>
       </c>
       <c r="K107" s="94">
         <v>0</v>
@@ -10340,7 +10306,7 @@
         <v>0</v>
       </c>
       <c r="Q107" s="94">
-        <v>20984</v>
+        <v>24911</v>
       </c>
     </row>
     <row r="108" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10365,7 +10331,7 @@
         <v>3725</v>
       </c>
       <c r="J108" s="21">
-        <v>0</v>
+        <v>3927</v>
       </c>
       <c r="K108" s="21">
         <v>0</v>
@@ -10386,7 +10352,7 @@
         <v>0</v>
       </c>
       <c r="Q108" s="21">
-        <v>20974</v>
+        <v>24901</v>
       </c>
     </row>
     <row r="109" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10411,7 +10377,7 @@
         <v>548</v>
       </c>
       <c r="J109" s="15">
-        <v>0</v>
+        <v>582</v>
       </c>
       <c r="K109" s="15">
         <v>0</v>
@@ -10432,7 +10398,7 @@
         <v>0</v>
       </c>
       <c r="Q109" s="15">
-        <v>2641</v>
+        <v>3223</v>
       </c>
     </row>
     <row r="110" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10503,7 +10469,7 @@
         <v>176</v>
       </c>
       <c r="J111" s="15">
-        <v>0</v>
+        <v>174</v>
       </c>
       <c r="K111" s="15">
         <v>0</v>
@@ -10524,7 +10490,7 @@
         <v>0</v>
       </c>
       <c r="Q111" s="15">
-        <v>979</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="112" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10549,7 +10515,7 @@
         <v>338</v>
       </c>
       <c r="J112" s="15">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="K112" s="15">
         <v>0</v>
@@ -10570,7 +10536,7 @@
         <v>0</v>
       </c>
       <c r="Q112" s="15">
-        <v>2478</v>
+        <v>2871</v>
       </c>
     </row>
     <row r="113" spans="2:17" s="1" customFormat="1" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -10641,7 +10607,7 @@
         <v>338</v>
       </c>
       <c r="J114" s="15">
-        <v>0</v>
+        <v>393</v>
       </c>
       <c r="K114" s="15">
         <v>0</v>
@@ -10662,7 +10628,7 @@
         <v>0</v>
       </c>
       <c r="Q114" s="15">
-        <v>2477</v>
+        <v>2870</v>
       </c>
     </row>
     <row r="115" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10687,7 +10653,7 @@
         <v>700</v>
       </c>
       <c r="J115" s="15">
-        <v>0</v>
+        <v>661</v>
       </c>
       <c r="K115" s="15">
         <v>0</v>
@@ -10708,7 +10674,7 @@
         <v>0</v>
       </c>
       <c r="Q115" s="15">
-        <v>5045</v>
+        <v>5706</v>
       </c>
     </row>
     <row r="116" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10733,7 +10699,7 @@
         <v>815</v>
       </c>
       <c r="J116" s="15">
-        <v>0</v>
+        <v>864</v>
       </c>
       <c r="K116" s="15">
         <v>0</v>
@@ -10754,7 +10720,7 @@
         <v>0</v>
       </c>
       <c r="Q116" s="15">
-        <v>4181</v>
+        <v>5045</v>
       </c>
     </row>
     <row r="117" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10779,7 +10745,7 @@
         <v>1148</v>
       </c>
       <c r="J117" s="15">
-        <v>0</v>
+        <v>1253</v>
       </c>
       <c r="K117" s="15">
         <v>0</v>
@@ -10800,7 +10766,7 @@
         <v>0</v>
       </c>
       <c r="Q117" s="15">
-        <v>5650</v>
+        <v>6903</v>
       </c>
     </row>
     <row r="118" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10871,7 +10837,7 @@
         <v>8223</v>
       </c>
       <c r="J119" s="93">
-        <v>0</v>
+        <v>7884</v>
       </c>
       <c r="K119" s="93">
         <v>0</v>
@@ -10892,7 +10858,7 @@
         <v>0</v>
       </c>
       <c r="Q119" s="93">
-        <v>44663</v>
+        <v>52547</v>
       </c>
     </row>
     <row r="120" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10917,7 +10883,7 @@
         <v>8176</v>
       </c>
       <c r="J120" s="21">
-        <v>0</v>
+        <v>7858</v>
       </c>
       <c r="K120" s="21">
         <v>0</v>
@@ -10938,7 +10904,7 @@
         <v>0</v>
       </c>
       <c r="Q120" s="21">
-        <v>44384</v>
+        <v>52242</v>
       </c>
     </row>
     <row r="121" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10963,7 +10929,7 @@
         <v>6</v>
       </c>
       <c r="J121" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K121" s="15">
         <v>0</v>
@@ -10984,7 +10950,7 @@
         <v>0</v>
       </c>
       <c r="Q121" s="15">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="122" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11009,7 +10975,7 @@
         <v>29</v>
       </c>
       <c r="J122" s="15">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K122" s="15">
         <v>0</v>
@@ -11030,7 +10996,7 @@
         <v>0</v>
       </c>
       <c r="Q122" s="15">
-        <v>150</v>
+        <v>175</v>
       </c>
     </row>
     <row r="123" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11055,7 +11021,7 @@
         <v>605</v>
       </c>
       <c r="J123" s="15">
-        <v>0</v>
+        <v>654</v>
       </c>
       <c r="K123" s="15">
         <v>0</v>
@@ -11076,7 +11042,7 @@
         <v>0</v>
       </c>
       <c r="Q123" s="15">
-        <v>2926</v>
+        <v>3580</v>
       </c>
     </row>
     <row r="124" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11101,7 +11067,7 @@
         <v>433</v>
       </c>
       <c r="J124" s="15">
-        <v>0</v>
+        <v>209</v>
       </c>
       <c r="K124" s="15">
         <v>0</v>
@@ -11122,7 +11088,7 @@
         <v>0</v>
       </c>
       <c r="Q124" s="15">
-        <v>2573</v>
+        <v>2782</v>
       </c>
     </row>
     <row r="125" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11147,7 +11113,7 @@
         <v>5</v>
       </c>
       <c r="J125" s="15">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K125" s="15">
         <v>0</v>
@@ -11168,7 +11134,7 @@
         <v>0</v>
       </c>
       <c r="Q125" s="15">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="126" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11193,7 +11159,7 @@
         <v>829</v>
       </c>
       <c r="J126" s="15">
-        <v>0</v>
+        <v>921</v>
       </c>
       <c r="K126" s="15">
         <v>0</v>
@@ -11214,7 +11180,7 @@
         <v>0</v>
       </c>
       <c r="Q126" s="15">
-        <v>4025</v>
+        <v>4946</v>
       </c>
     </row>
     <row r="127" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11239,7 +11205,7 @@
         <v>2202</v>
       </c>
       <c r="J127" s="15">
-        <v>0</v>
+        <v>1972</v>
       </c>
       <c r="K127" s="15">
         <v>0</v>
@@ -11260,7 +11226,7 @@
         <v>0</v>
       </c>
       <c r="Q127" s="15">
-        <v>11438</v>
+        <v>13410</v>
       </c>
     </row>
     <row r="128" spans="2:17" s="1" customFormat="1" ht="19.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -11377,7 +11343,7 @@
         <v>1586</v>
       </c>
       <c r="J130" s="15">
-        <v>0</v>
+        <v>1417</v>
       </c>
       <c r="K130" s="15">
         <v>0</v>
@@ -11398,7 +11364,7 @@
         <v>0</v>
       </c>
       <c r="Q130" s="15">
-        <v>10577</v>
+        <v>11994</v>
       </c>
     </row>
     <row r="131" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11423,7 +11389,7 @@
         <v>209</v>
       </c>
       <c r="J131" s="15">
-        <v>0</v>
+        <v>206</v>
       </c>
       <c r="K131" s="15">
         <v>0</v>
@@ -11444,7 +11410,7 @@
         <v>0</v>
       </c>
       <c r="Q131" s="15">
-        <v>984</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="132" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11469,7 +11435,7 @@
         <v>6</v>
       </c>
       <c r="J132" s="15">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="K132" s="15">
         <v>0</v>
@@ -11490,7 +11456,7 @@
         <v>0</v>
       </c>
       <c r="Q132" s="15">
-        <v>27</v>
+        <v>44</v>
       </c>
     </row>
     <row r="133" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11515,7 +11481,7 @@
         <v>5</v>
       </c>
       <c r="J133" s="15">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K133" s="15">
         <v>0</v>
@@ -11536,7 +11502,7 @@
         <v>0</v>
       </c>
       <c r="Q133" s="15">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="134" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11561,7 +11527,7 @@
         <v>1</v>
       </c>
       <c r="J134" s="15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K134" s="15">
         <v>0</v>
@@ -11582,7 +11548,7 @@
         <v>0</v>
       </c>
       <c r="Q134" s="15">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="135" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11607,7 +11573,7 @@
         <v>815</v>
       </c>
       <c r="J135" s="15">
-        <v>0</v>
+        <v>864</v>
       </c>
       <c r="K135" s="15">
         <v>0</v>
@@ -11628,7 +11594,7 @@
         <v>0</v>
       </c>
       <c r="Q135" s="15">
-        <v>4181</v>
+        <v>5045</v>
       </c>
     </row>
     <row r="136" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11653,7 +11619,7 @@
         <v>1451</v>
       </c>
       <c r="J136" s="15">
-        <v>0</v>
+        <v>1562</v>
       </c>
       <c r="K136" s="15">
         <v>0</v>
@@ -11674,7 +11640,7 @@
         <v>0</v>
       </c>
       <c r="Q136" s="15">
-        <v>7449</v>
+        <v>9011</v>
       </c>
     </row>
     <row r="137" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11699,7 +11665,7 @@
         <v>47</v>
       </c>
       <c r="J137" s="43">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="K137" s="43">
         <v>0</v>
@@ -11720,7 +11686,7 @@
         <v>0</v>
       </c>
       <c r="Q137" s="43">
-        <v>279</v>
+        <v>305</v>
       </c>
     </row>
     <row r="138" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11745,7 +11711,7 @@
         <v>1920</v>
       </c>
       <c r="J138" s="93">
-        <v>0</v>
+        <v>1774</v>
       </c>
       <c r="K138" s="93">
         <v>0</v>
@@ -11766,7 +11732,7 @@
         <v>0</v>
       </c>
       <c r="Q138" s="93">
-        <v>9548</v>
+        <v>11322</v>
       </c>
     </row>
     <row r="139" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11791,7 +11757,7 @@
         <v>1916</v>
       </c>
       <c r="J139" s="21">
-        <v>0</v>
+        <v>1774</v>
       </c>
       <c r="K139" s="21">
         <v>0</v>
@@ -11812,7 +11778,7 @@
         <v>0</v>
       </c>
       <c r="Q139" s="21">
-        <v>9511</v>
+        <v>11285</v>
       </c>
     </row>
     <row r="140" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11837,7 +11803,7 @@
         <v>195</v>
       </c>
       <c r="J140" s="15">
-        <v>0</v>
+        <v>267</v>
       </c>
       <c r="K140" s="15">
         <v>0</v>
@@ -11858,7 +11824,7 @@
         <v>0</v>
       </c>
       <c r="Q140" s="15">
-        <v>1468</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="141" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11883,7 +11849,7 @@
         <v>128</v>
       </c>
       <c r="J141" s="15">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="K141" s="15">
         <v>0</v>
@@ -11904,7 +11870,7 @@
         <v>0</v>
       </c>
       <c r="Q141" s="15">
-        <v>263</v>
+        <v>315</v>
       </c>
     </row>
     <row r="142" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11929,7 +11895,7 @@
         <v>439</v>
       </c>
       <c r="J142" s="15">
-        <v>0</v>
+        <v>345</v>
       </c>
       <c r="K142" s="15">
         <v>0</v>
@@ -11950,7 +11916,7 @@
         <v>0</v>
       </c>
       <c r="Q142" s="15">
-        <v>2642</v>
+        <v>2987</v>
       </c>
     </row>
     <row r="143" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11975,7 +11941,7 @@
         <v>1060</v>
       </c>
       <c r="J143" s="15">
-        <v>0</v>
+        <v>1021</v>
       </c>
       <c r="K143" s="15">
         <v>0</v>
@@ -11996,7 +11962,7 @@
         <v>0</v>
       </c>
       <c r="Q143" s="15">
-        <v>4602</v>
+        <v>5623</v>
       </c>
     </row>
     <row r="144" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12021,7 +11987,7 @@
         <v>20</v>
       </c>
       <c r="J144" s="15">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K144" s="15">
         <v>0</v>
@@ -12042,7 +12008,7 @@
         <v>0</v>
       </c>
       <c r="Q144" s="15">
-        <v>100</v>
+        <v>123</v>
       </c>
     </row>
     <row r="145" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12067,7 +12033,7 @@
         <v>74</v>
       </c>
       <c r="J145" s="15">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="K145" s="15">
         <v>0</v>
@@ -12088,7 +12054,7 @@
         <v>0</v>
       </c>
       <c r="Q145" s="15">
-        <v>436</v>
+        <v>502</v>
       </c>
     </row>
     <row r="146" spans="2:17" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12151,7 +12117,7 @@
   <dimension ref="B2:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12293,7 +12259,7 @@
         <v>44342</v>
       </c>
       <c r="I7" s="20">
-        <v>0</v>
+        <v>36622</v>
       </c>
       <c r="J7" s="20">
         <v>0</v>
@@ -12314,7 +12280,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="20">
-        <v>190595</v>
+        <v>227217</v>
       </c>
       <c r="Q7" s="3"/>
     </row>
@@ -12339,7 +12305,7 @@
         <v>42614</v>
       </c>
       <c r="I8" s="21">
-        <v>0</v>
+        <v>34550</v>
       </c>
       <c r="J8" s="21">
         <v>0</v>
@@ -12360,7 +12326,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="21">
-        <v>182256</v>
+        <v>216806</v>
       </c>
       <c r="Q8" s="3"/>
     </row>
@@ -12385,7 +12351,7 @@
         <v>35288</v>
       </c>
       <c r="I9" s="15">
-        <v>0</v>
+        <v>27583</v>
       </c>
       <c r="J9" s="15">
         <v>0</v>
@@ -12406,7 +12372,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="15">
-        <v>153028</v>
+        <v>180611</v>
       </c>
       <c r="Q9" s="3"/>
     </row>
@@ -12431,7 +12397,7 @@
         <v>7326</v>
       </c>
       <c r="I10" s="15">
-        <v>0</v>
+        <v>6967</v>
       </c>
       <c r="J10" s="15">
         <v>0</v>
@@ -12452,7 +12418,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="15">
-        <v>29228</v>
+        <v>36195</v>
       </c>
       <c r="Q10" s="3"/>
     </row>
@@ -12477,7 +12443,7 @@
         <v>1304</v>
       </c>
       <c r="I11" s="21">
-        <v>0</v>
+        <v>1389</v>
       </c>
       <c r="J11" s="21">
         <v>0</v>
@@ -12498,7 +12464,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="21">
-        <v>6773</v>
+        <v>8162</v>
       </c>
       <c r="Q11" s="3"/>
     </row>
@@ -12523,7 +12489,7 @@
         <v>85</v>
       </c>
       <c r="I12" s="15">
-        <v>0</v>
+        <v>146</v>
       </c>
       <c r="J12" s="15">
         <v>0</v>
@@ -12544,7 +12510,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="15">
-        <v>436</v>
+        <v>582</v>
       </c>
       <c r="Q12" s="3"/>
     </row>
@@ -12569,7 +12535,7 @@
         <v>155</v>
       </c>
       <c r="I13" s="15">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="J13" s="15">
         <v>0</v>
@@ -12590,7 +12556,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="15">
-        <v>972</v>
+        <v>1065</v>
       </c>
       <c r="Q13" s="3"/>
     </row>
@@ -12615,7 +12581,7 @@
         <v>12</v>
       </c>
       <c r="I14" s="15">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J14" s="15">
         <v>0</v>
@@ -12636,7 +12602,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="15">
-        <v>418</v>
+        <v>431</v>
       </c>
       <c r="Q14" s="3"/>
     </row>
@@ -12661,7 +12627,7 @@
         <v>450</v>
       </c>
       <c r="I15" s="15">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="J15" s="15">
         <v>0</v>
@@ -12682,7 +12648,7 @@
         <v>0</v>
       </c>
       <c r="P15" s="15">
-        <v>1931</v>
+        <v>2306</v>
       </c>
       <c r="Q15" s="3"/>
     </row>
@@ -12707,7 +12673,7 @@
         <v>602</v>
       </c>
       <c r="I16" s="15">
-        <v>0</v>
+        <v>762</v>
       </c>
       <c r="J16" s="15">
         <v>0</v>
@@ -12728,7 +12694,7 @@
         <v>0</v>
       </c>
       <c r="P16" s="15">
-        <v>3016</v>
+        <v>3778</v>
       </c>
       <c r="Q16" s="3"/>
     </row>
@@ -12753,7 +12719,7 @@
         <v>424</v>
       </c>
       <c r="I17" s="21">
-        <v>0</v>
+        <v>683</v>
       </c>
       <c r="J17" s="21">
         <v>0</v>
@@ -12774,7 +12740,7 @@
         <v>0</v>
       </c>
       <c r="P17" s="21">
-        <v>1566</v>
+        <v>2249</v>
       </c>
       <c r="Q17" s="3"/>
     </row>
@@ -12799,7 +12765,7 @@
         <v>160</v>
       </c>
       <c r="I18" s="42">
-        <v>0</v>
+        <v>322</v>
       </c>
       <c r="J18" s="42">
         <v>0</v>
@@ -12820,7 +12786,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="15">
-        <v>575</v>
+        <v>897</v>
       </c>
       <c r="Q18" s="3"/>
     </row>
@@ -12845,7 +12811,7 @@
         <v>264</v>
       </c>
       <c r="I19" s="41">
-        <v>0</v>
+        <v>361</v>
       </c>
       <c r="J19" s="41">
         <v>0</v>
@@ -12866,7 +12832,7 @@
         <v>0</v>
       </c>
       <c r="P19" s="33">
-        <v>991</v>
+        <v>1352</v>
       </c>
       <c r="Q19" s="3"/>
     </row>
@@ -12884,7 +12850,7 @@
   <dimension ref="B3:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13026,7 +12992,7 @@
         <v>227914</v>
       </c>
       <c r="I8" s="20">
-        <v>0</v>
+        <v>189182</v>
       </c>
       <c r="J8" s="20">
         <v>0</v>
@@ -13047,7 +13013,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="20">
-        <v>942786</v>
+        <v>1131968</v>
       </c>
       <c r="Q8" s="3"/>
     </row>
@@ -13072,7 +13038,7 @@
         <v>217575</v>
       </c>
       <c r="I9" s="21">
-        <v>0</v>
+        <v>180204</v>
       </c>
       <c r="J9" s="21">
         <v>0</v>
@@ -13093,7 +13059,7 @@
         <v>0</v>
       </c>
       <c r="P9" s="21">
-        <v>895052</v>
+        <v>1075256</v>
       </c>
       <c r="Q9" s="3"/>
     </row>
@@ -13118,7 +13084,7 @@
         <v>175051</v>
       </c>
       <c r="I10" s="15">
-        <v>0</v>
+        <v>142612</v>
       </c>
       <c r="J10" s="15">
         <v>0</v>
@@ -13139,7 +13105,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="15">
-        <v>729016</v>
+        <v>871628</v>
       </c>
       <c r="Q10" s="3"/>
     </row>
@@ -13164,7 +13130,7 @@
         <v>42524</v>
       </c>
       <c r="I11" s="15">
-        <v>0</v>
+        <v>37592</v>
       </c>
       <c r="J11" s="15">
         <v>0</v>
@@ -13185,7 +13151,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="15">
-        <v>166036</v>
+        <v>203628</v>
       </c>
       <c r="Q11" s="3"/>
     </row>
@@ -13210,7 +13176,7 @@
         <v>8392</v>
       </c>
       <c r="I12" s="21">
-        <v>0</v>
+        <v>7029</v>
       </c>
       <c r="J12" s="21">
         <v>0</v>
@@ -13231,7 +13197,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="21">
-        <v>40144</v>
+        <v>47173</v>
       </c>
       <c r="Q12" s="3"/>
     </row>
@@ -13256,7 +13222,7 @@
         <v>73</v>
       </c>
       <c r="I13" s="15">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="J13" s="15">
         <v>0</v>
@@ -13277,7 +13243,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="15">
-        <v>699</v>
+        <v>734</v>
       </c>
       <c r="Q13" s="3"/>
     </row>
@@ -13302,7 +13268,7 @@
         <v>1202</v>
       </c>
       <c r="I14" s="15">
-        <v>0</v>
+        <v>758</v>
       </c>
       <c r="J14" s="15">
         <v>0</v>
@@ -13323,7 +13289,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="15">
-        <v>6478</v>
+        <v>7236</v>
       </c>
       <c r="Q14" s="3"/>
     </row>
@@ -13348,7 +13314,7 @@
         <v>169</v>
       </c>
       <c r="I15" s="15">
-        <v>0</v>
+        <v>117</v>
       </c>
       <c r="J15" s="15">
         <v>0</v>
@@ -13369,7 +13335,7 @@
         <v>0</v>
       </c>
       <c r="P15" s="15">
-        <v>1358</v>
+        <v>1475</v>
       </c>
       <c r="Q15" s="3"/>
     </row>
@@ -13394,7 +13360,7 @@
         <v>2451</v>
       </c>
       <c r="I16" s="15">
-        <v>0</v>
+        <v>2083</v>
       </c>
       <c r="J16" s="15">
         <v>0</v>
@@ -13415,7 +13381,7 @@
         <v>0</v>
       </c>
       <c r="P16" s="15">
-        <v>11182</v>
+        <v>13265</v>
       </c>
       <c r="Q16" s="3"/>
     </row>
@@ -13440,7 +13406,7 @@
         <v>4497</v>
       </c>
       <c r="I17" s="15">
-        <v>0</v>
+        <v>4036</v>
       </c>
       <c r="J17" s="15">
         <v>0</v>
@@ -13461,7 +13427,7 @@
         <v>0</v>
       </c>
       <c r="P17" s="15">
-        <v>20427</v>
+        <v>24463</v>
       </c>
       <c r="Q17" s="3"/>
     </row>
@@ -13486,7 +13452,7 @@
         <v>1947</v>
       </c>
       <c r="I18" s="21">
-        <v>0</v>
+        <v>1949</v>
       </c>
       <c r="J18" s="21">
         <v>0</v>
@@ -13507,7 +13473,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="21">
-        <v>7590</v>
+        <v>9539</v>
       </c>
       <c r="Q18" s="3"/>
     </row>
@@ -13532,7 +13498,7 @@
         <v>415</v>
       </c>
       <c r="I19" s="42">
-        <v>0</v>
+        <v>518</v>
       </c>
       <c r="J19" s="42">
         <v>0</v>
@@ -13553,7 +13519,7 @@
         <v>0</v>
       </c>
       <c r="P19" s="15">
-        <v>1106</v>
+        <v>1624</v>
       </c>
       <c r="Q19" s="3"/>
     </row>
@@ -13578,7 +13544,7 @@
         <v>1532</v>
       </c>
       <c r="I20" s="41">
-        <v>0</v>
+        <v>1431</v>
       </c>
       <c r="J20" s="41">
         <v>0</v>
@@ -13599,7 +13565,7 @@
         <v>0</v>
       </c>
       <c r="P20" s="33">
-        <v>6484</v>
+        <v>7915</v>
       </c>
       <c r="Q20" s="3"/>
     </row>
@@ -13616,8 +13582,8 @@
   </sheetPr>
   <dimension ref="B2:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13761,7 +13727,7 @@
         <v>1578</v>
       </c>
       <c r="I7" s="20">
-        <v>0</v>
+        <v>1367</v>
       </c>
       <c r="J7" s="20">
         <v>0</v>
@@ -13782,7 +13748,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="20">
-        <v>7196</v>
+        <v>8563</v>
       </c>
       <c r="Q7" s="3"/>
     </row>
@@ -13945,7 +13911,7 @@
         <v>1193</v>
       </c>
       <c r="I11" s="21">
-        <v>0</v>
+        <v>956</v>
       </c>
       <c r="J11" s="21">
         <v>0</v>
@@ -13966,7 +13932,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="21">
-        <v>5870</v>
+        <v>6826</v>
       </c>
       <c r="Q11" s="3"/>
     </row>
@@ -13991,7 +13957,7 @@
         <v>385</v>
       </c>
       <c r="I12" s="43">
-        <v>0</v>
+        <v>411</v>
       </c>
       <c r="J12" s="43">
         <v>0</v>
@@ -14012,7 +13978,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="43">
-        <v>1326</v>
+        <v>1737</v>
       </c>
       <c r="Q12" s="3"/>
     </row>
@@ -14111,7 +14077,7 @@
         <v>1065524.6395590352</v>
       </c>
       <c r="I21" s="106">
-        <v>0</v>
+        <v>1001109.4199487215</v>
       </c>
       <c r="J21" s="106">
         <v>0</v>
@@ -14132,7 +14098,7 @@
         <v>0</v>
       </c>
       <c r="P21" s="106">
-        <v>4741422.2896819953</v>
+        <v>5742531.7096307166</v>
       </c>
     </row>
     <row r="25" spans="2:17" ht="23.25" x14ac:dyDescent="0.25">
@@ -14228,7 +14194,7 @@
         <v>100181</v>
       </c>
       <c r="I30" s="106">
-        <v>0</v>
+        <v>99676</v>
       </c>
       <c r="J30" s="106">
         <v>0</v>

</xml_diff>